<commit_message>
add buff define realize
</commit_message>
<xml_diff>
--- a/Data/BuffDefine.xlsx
+++ b/Data/BuffDefine.xlsx
@@ -1312,8 +1312,8 @@
   <sheetPr/>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>

<commit_message>
add black bar manager
</commit_message>
<xml_diff>
--- a/Data/BuffDefine.xlsx
+++ b/Data/BuffDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -195,6 +195,30 @@
   </si>
   <si>
     <t>增加闪避率</t>
+  </si>
+  <si>
+    <t>沉默</t>
+  </si>
+  <si>
+    <t>Silent</t>
+  </si>
+  <si>
+    <t>buff_silent_icon</t>
+  </si>
+  <si>
+    <t>沉默的单位无法进行攻击</t>
+  </si>
+  <si>
+    <t>禁锢</t>
+  </si>
+  <si>
+    <t>Confine</t>
+  </si>
+  <si>
+    <t>buff_confine_icon</t>
+  </si>
+  <si>
+    <t>禁锢的单位无法移动</t>
   </si>
 </sst>
 </file>
@@ -1349,10 +1373,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1821,6 +1845,76 @@
         <v>55</v>
       </c>
     </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add buff icon & treasure display
</commit_message>
<xml_diff>
--- a/Data/BuffDefine.xlsx
+++ b/Data/BuffDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -92,76 +92,79 @@
     <t>Trauma</t>
   </si>
   <si>
+    <t>buff_Trauma_icon</t>
+  </si>
+  <si>
+    <t>拥有外伤状态的角色受到伤害时，额外受到外伤层数的伤害</t>
+  </si>
+  <si>
+    <t>念力</t>
+  </si>
+  <si>
+    <t>MentalPower</t>
+  </si>
+  <si>
+    <t>buff_mentalPower_icon</t>
+  </si>
+  <si>
+    <t>拥有念力的角色在进行攻击时，额外造成念力层数的伤害</t>
+  </si>
+  <si>
+    <t>腐蚀</t>
+  </si>
+  <si>
+    <t>Corrosion</t>
+  </si>
+  <si>
+    <t>buff_corrosion_icon</t>
+  </si>
+  <si>
+    <t>拥有腐蚀状态的角色回合开始时受到一次腐蚀层数的伤害</t>
+  </si>
+  <si>
+    <t>眩晕</t>
+  </si>
+  <si>
+    <t>Dizzy</t>
+  </si>
+  <si>
+    <t>buff_dizzy_icon</t>
+  </si>
+  <si>
+    <t>眩晕的角色行动时会跳过自身回合，然后眩晕层数减1</t>
+  </si>
+  <si>
+    <t>灼伤</t>
+  </si>
+  <si>
+    <t>Burning</t>
+  </si>
+  <si>
+    <t>buff_burning_icon</t>
+  </si>
+  <si>
+    <t>灼伤在角色回合开始时，造成一次伤害（受施加者属性影响）</t>
+  </si>
+  <si>
+    <t>减防</t>
+  </si>
+  <si>
+    <t>ChangeProperty</t>
+  </si>
+  <si>
+    <t>buff_decreaseDefense_icon</t>
+  </si>
+  <si>
+    <t>防御降低</t>
+  </si>
+  <si>
+    <t>流血</t>
+  </si>
+  <si>
+    <t>Bleeding</t>
+  </si>
+  <si>
     <t>buff_bleeding_icon</t>
-  </si>
-  <si>
-    <t>拥有外伤状态的角色受到伤害时，额外受到外伤层数的伤害</t>
-  </si>
-  <si>
-    <t>念力</t>
-  </si>
-  <si>
-    <t>MentalPower</t>
-  </si>
-  <si>
-    <t>buff_mentalPower_icon</t>
-  </si>
-  <si>
-    <t>拥有念力的角色在进行攻击时，额外造成念力层数的伤害</t>
-  </si>
-  <si>
-    <t>腐蚀</t>
-  </si>
-  <si>
-    <t>Corrosion</t>
-  </si>
-  <si>
-    <t>buff_corrosion_icon</t>
-  </si>
-  <si>
-    <t>拥有腐蚀状态的角色回合开始时受到一次腐蚀层数的伤害</t>
-  </si>
-  <si>
-    <t>眩晕</t>
-  </si>
-  <si>
-    <t>Dizzy</t>
-  </si>
-  <si>
-    <t>buff_dizzy_icon</t>
-  </si>
-  <si>
-    <t>眩晕的角色行动时会跳过自身回合，然后眩晕层数减1</t>
-  </si>
-  <si>
-    <t>灼伤</t>
-  </si>
-  <si>
-    <t>Burning</t>
-  </si>
-  <si>
-    <t>buff_burning_icon</t>
-  </si>
-  <si>
-    <t>灼伤在角色回合开始时，造成一次伤害（受施加者属性影响）</t>
-  </si>
-  <si>
-    <t>减防</t>
-  </si>
-  <si>
-    <t>ChangeProperty</t>
-  </si>
-  <si>
-    <t>buff_decreaseDefense_icon</t>
-  </si>
-  <si>
-    <t>防御降低</t>
-  </si>
-  <si>
-    <t>流血</t>
-  </si>
-  <si>
-    <t>Bleeding</t>
   </si>
   <si>
     <t>拥有流血状态的角色移动时，受到流血层数*移动步数的伤害</t>
@@ -1376,7 +1379,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1734,10 +1737,10 @@
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1745,7 +1748,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1769,10 +1772,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1780,10 +1783,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1804,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1815,7 +1818,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -1839,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1850,10 +1853,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>-1</v>
@@ -1874,10 +1877,10 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1885,10 +1888,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>-1</v>
@@ -1909,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change character property & team window bug remain
</commit_message>
<xml_diff>
--- a/Data/BuffDefine.xlsx
+++ b/Data/BuffDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -62,18 +62,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>虚无</t>
-  </si>
-  <si>
-    <t>Nothingness</t>
-  </si>
-  <si>
-    <t>buff_nothingness_icon</t>
-  </si>
-  <si>
-    <t>每当拥有虚无状态的角色回合结束，叠加一层，当叠加至五层时，立即堕入虚无（生命值归零）,对精英敌人则造成一次真实伤害</t>
-  </si>
-  <si>
     <t>隐身</t>
   </si>
   <si>
@@ -146,54 +134,36 @@
     <t>灼伤在角色回合开始时，造成一次伤害（受施加者属性影响）</t>
   </si>
   <si>
-    <t>减防</t>
+    <t>流血</t>
+  </si>
+  <si>
+    <t>Bleeding</t>
+  </si>
+  <si>
+    <t>buff_bleeding_icon</t>
+  </si>
+  <si>
+    <t>拥有流血状态的角色移动时，受到流血层数*移动步数的伤害</t>
+  </si>
+  <si>
+    <t>无敌</t>
+  </si>
+  <si>
+    <t>Invincible</t>
+  </si>
+  <si>
+    <t>buff_invincible_icon</t>
+  </si>
+  <si>
+    <t>免疫所有伤害</t>
+  </si>
+  <si>
+    <t>闪避</t>
   </si>
   <si>
     <t>ChangeProperty</t>
   </si>
   <si>
-    <t>buff_decreaseDefense_icon</t>
-  </si>
-  <si>
-    <t>防御降低</t>
-  </si>
-  <si>
-    <t>流血</t>
-  </si>
-  <si>
-    <t>Bleeding</t>
-  </si>
-  <si>
-    <t>buff_bleeding_icon</t>
-  </si>
-  <si>
-    <t>拥有流血状态的角色移动时，受到流血层数*移动步数的伤害</t>
-  </si>
-  <si>
-    <t>减伤</t>
-  </si>
-  <si>
-    <t>buff_protection_icon</t>
-  </si>
-  <si>
-    <t>伤害减免</t>
-  </si>
-  <si>
-    <t>无敌</t>
-  </si>
-  <si>
-    <t>Invincible</t>
-  </si>
-  <si>
-    <t>buff_invincible_icon</t>
-  </si>
-  <si>
-    <t>免疫所有伤害</t>
-  </si>
-  <si>
-    <t>闪避</t>
-  </si>
-  <si>
     <t>buff_dodge_icon</t>
   </si>
   <si>
@@ -222,6 +192,39 @@
   </si>
   <si>
     <t>禁锢的单位无法移动</t>
+  </si>
+  <si>
+    <t>力竭</t>
+  </si>
+  <si>
+    <t>Exhaustion</t>
+  </si>
+  <si>
+    <t>虚弱</t>
+  </si>
+  <si>
+    <t>Weakness</t>
+  </si>
+  <si>
+    <t>破绽</t>
+  </si>
+  <si>
+    <t>Flaw</t>
+  </si>
+  <si>
+    <t>连击</t>
+  </si>
+  <si>
+    <t>Batter</t>
+  </si>
+  <si>
+    <t>反击</t>
+  </si>
+  <si>
+    <t>锋锐</t>
+  </si>
+  <si>
+    <t>Sharp</t>
   </si>
 </sst>
 </file>
@@ -1376,10 +1379,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1445,16 +1448,16 @@
         <v>-1</v>
       </c>
       <c r="F2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1480,16 +1483,16 @@
         <v>-1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1505,7 +1508,7 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4">
@@ -1526,7 +1529,7 @@
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K4" t="s">
@@ -1550,13 +1553,13 @@
         <v>-1</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -1575,7 +1578,7 @@
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
       <c r="D6">
@@ -1585,7 +1588,7 @@
         <v>-1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1594,9 +1597,9 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
         <v>29</v>
       </c>
       <c r="K6" t="s">
@@ -1610,7 +1613,7 @@
       <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D7">
@@ -1620,7 +1623,7 @@
         <v>-1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1629,9 +1632,9 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K7" t="s">
@@ -1645,7 +1648,7 @@
       <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8">
@@ -1655,18 +1658,18 @@
         <v>-1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
         <v>37</v>
       </c>
       <c r="K8" t="s">
@@ -1684,22 +1687,22 @@
         <v>40</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="E9">
-        <v>-10</v>
+        <v>-1</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="s">
         <v>41</v>
@@ -1719,22 +1722,22 @@
         <v>44</v>
       </c>
       <c r="D10">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="F10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J10" t="s">
         <v>45</v>
@@ -1751,16 +1754,16 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1769,13 +1772,13 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1783,10 +1786,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1801,16 +1804,16 @@
         <v>2</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1818,16 +1821,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1836,16 +1839,16 @@
         <v>2</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" t="s">
         <v>55</v>
-      </c>
-      <c r="K13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1877,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1888,10 +1891,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15">
         <v>-1</v>
@@ -1912,9 +1915,79 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" t="s">
         <v>63</v>
       </c>
-      <c r="K15" t="s">
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>